<commit_message>
Fixed error in bonds price calculation from yield
</commit_message>
<xml_diff>
--- a/misc analysis/Correlation from Portvisualizer.xlsx
+++ b/misc analysis/Correlation from Portvisualizer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feder\Desktop\portfolio-allocation\misc analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feder\Desktop\Git_Repos\portfolio-allocation\misc analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C9332A-DE95-4726-8F1B-AB5386DD149F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197A0AAA-1CB3-472D-B9F6-1895EC73067B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{C1EC8239-D76C-4B1B-817A-9402BE5BCB19}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -806,45 +806,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936F9293-0876-43FA-8AA4-D9BE0EABDCE6}">
   <dimension ref="A1:AK83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W5" sqref="W5:AJ5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.86328125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="5.86328125" style="4" customWidth="1"/>
-    <col min="3" max="16" width="8.1328125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="8.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.86328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" style="4" customWidth="1"/>
+    <col min="3" max="16" width="8.140625" style="4" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.73046875" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="9" style="4"/>
-    <col min="23" max="24" width="4.265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.59765625" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.73046875" style="4" bestFit="1" customWidth="1"/>
-    <col min="28" max="36" width="4.265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.1328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="4.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="36" width="4.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="38" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="3" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:36" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="11.65" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" ht="12" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>39</v>
       </c>
@@ -878,7 +878,7 @@
       <c r="S4" s="17"/>
       <c r="T4" s="17"/>
     </row>
-    <row r="5" spans="1:36" ht="40.9" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" ht="57" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -939,22 +939,50 @@
       <c r="T5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="6"/>
-      <c r="AA5" s="6"/>
-      <c r="AB5" s="6"/>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="6"/>
-      <c r="AE5" s="6"/>
-      <c r="AF5" s="6"/>
-      <c r="AG5" s="6"/>
-      <c r="AH5" s="6"/>
-      <c r="AI5" s="6"/>
-      <c r="AJ5" s="6"/>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="W5" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="X5" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y5" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z5" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA5" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB5" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC5" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD5" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE5" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF5" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG5" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH5" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI5" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ5" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
@@ -1029,7 +1057,7 @@
       <c r="AH6" s="14"/>
       <c r="AI6" s="14"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>22</v>
       </c>
@@ -1091,7 +1119,7 @@
         <v>0.15909999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
@@ -1153,7 +1181,7 @@
         <v>0.18060000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>29</v>
       </c>
@@ -1215,7 +1243,7 @@
         <v>0.1653</v>
       </c>
     </row>
-    <row r="10" spans="1:36" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>30</v>
       </c>
@@ -1279,7 +1307,7 @@
       <c r="Y10" s="18"/>
       <c r="AA10" s="18"/>
     </row>
-    <row r="11" spans="1:36" ht="20.65" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:36" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>31</v>
       </c>
@@ -1354,7 +1382,7 @@
       <c r="AH11" s="14"/>
       <c r="AI11" s="14"/>
     </row>
-    <row r="12" spans="1:36" ht="10.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
@@ -1417,7 +1445,7 @@
       </c>
       <c r="AA12" s="19"/>
     </row>
-    <row r="13" spans="1:36" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>24</v>
       </c>
@@ -1479,7 +1507,7 @@
         <v>9.7000000000000003E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>25</v>
       </c>
@@ -1541,7 +1569,7 @@
         <v>3.1800000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:36" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>26</v>
       </c>
@@ -1603,7 +1631,7 @@
         <v>0.12770000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>28</v>
       </c>
@@ -1665,7 +1693,7 @@
         <v>4.6399999999999997E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>27</v>
       </c>
@@ -1727,7 +1755,7 @@
         <v>4.5199999999999997E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>33</v>
       </c>
@@ -1789,7 +1817,7 @@
         <v>0.1757</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>34</v>
       </c>
@@ -1851,7 +1879,7 @@
         <v>0.16520000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="11"/>
@@ -1873,7 +1901,7 @@
       <c r="S20" s="12"/>
       <c r="T20" s="12"/>
     </row>
-    <row r="21" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>36</v>
       </c>
@@ -1902,7 +1930,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:36" ht="40.9" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:36" ht="57" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>0</v>
       </c>
@@ -2009,7 +2037,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>20</v>
       </c>
@@ -2130,7 +2158,7 @@
         <v>-6.0000000000000005E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>22</v>
       </c>
@@ -2251,7 +2279,7 @@
         <v>-0.06</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>23</v>
       </c>
@@ -2372,7 +2400,7 @@
         <v>-3.9999999999999994E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:36" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
         <v>29</v>
       </c>
@@ -2493,7 +2521,7 @@
         <v>-7.9999999999999988E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:36" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>30</v>
       </c>
@@ -2614,7 +2642,7 @@
         <v>-9.0000000000000024E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:36" ht="20.65" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:36" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>31</v>
       </c>
@@ -2735,7 +2763,7 @@
         <v>-0.16</v>
       </c>
     </row>
-    <row r="29" spans="1:36" ht="10.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>32</v>
       </c>
@@ -2856,7 +2884,7 @@
         <v>-7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:36" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
         <v>24</v>
       </c>
@@ -2977,7 +3005,7 @@
         <v>-0.14000000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>25</v>
       </c>
@@ -3098,7 +3126,7 @@
         <v>-0.18</v>
       </c>
     </row>
-    <row r="32" spans="1:36" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:36" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
         <v>26</v>
       </c>
@@ -3219,7 +3247,7 @@
         <v>-0.03</v>
       </c>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:37" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>28</v>
       </c>
@@ -3340,7 +3368,7 @@
         <v>-0.09</v>
       </c>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
         <v>27</v>
       </c>
@@ -3461,7 +3489,7 @@
         <v>-0.23000000000000004</v>
       </c>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:37" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>33</v>
       </c>
@@ -3586,7 +3614,7 @@
         <v>-0.39</v>
       </c>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
         <v>34</v>
       </c>
@@ -3711,12 +3739,12 @@
         <v>0.21999999999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:37" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="16"/>
       <c r="B39" s="17"/>
       <c r="C39" s="41" t="s">
@@ -3763,7 +3791,7 @@
       <c r="AI39" s="6"/>
       <c r="AJ39" s="6"/>
     </row>
-    <row r="40" spans="1:37" ht="40.9" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:37" ht="57" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>0</v>
       </c>
@@ -3870,7 +3898,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:37" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>20</v>
       </c>
@@ -3991,7 +4019,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="42" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
         <v>22</v>
       </c>
@@ -4112,7 +4140,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="43" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>23</v>
       </c>
@@ -4233,7 +4261,7 @@
         <v>9.999999999999995E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:37" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:37" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
         <v>29</v>
       </c>
@@ -4354,7 +4382,7 @@
         <v>-4.0000000000000008E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:37" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:37" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>30</v>
       </c>
@@ -4475,7 +4503,7 @@
         <v>-1.9999999999999962E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:37" ht="20.65" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:37" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>31</v>
       </c>
@@ -4596,7 +4624,7 @@
         <v>-0.26999999999999996</v>
       </c>
     </row>
-    <row r="47" spans="1:37" ht="10.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:37" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>32</v>
       </c>
@@ -4717,7 +4745,7 @@
         <v>-0.38</v>
       </c>
     </row>
-    <row r="48" spans="1:37" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:37" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
         <v>24</v>
       </c>
@@ -4838,7 +4866,7 @@
         <v>-0.22999999999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:37" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>25</v>
       </c>
@@ -4959,7 +4987,7 @@
         <v>-0.33</v>
       </c>
     </row>
-    <row r="50" spans="1:37" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:37" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
         <v>26</v>
       </c>
@@ -5080,7 +5108,7 @@
         <v>-0.27</v>
       </c>
     </row>
-    <row r="51" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:37" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>28</v>
       </c>
@@ -5201,7 +5229,7 @@
         <v>-7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
         <v>27</v>
       </c>
@@ -5323,7 +5351,7 @@
       </c>
       <c r="AK52" s="8"/>
     </row>
-    <row r="53" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:37" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
         <v>33</v>
       </c>
@@ -5448,7 +5476,7 @@
         <v>-0.69</v>
       </c>
     </row>
-    <row r="54" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
         <v>34</v>
       </c>
@@ -5573,12 +5601,12 @@
         <v>0.42000000000000004</v>
       </c>
     </row>
-    <row r="58" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="67" spans="1:21" ht="71.650000000000006" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:21" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="34" t="s">
         <v>0</v>
       </c>
@@ -5643,7 +5671,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:21" ht="28.5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:21" ht="30" x14ac:dyDescent="0.2">
       <c r="A68" s="36" t="s">
         <v>20</v>
       </c>
@@ -5708,7 +5736,7 @@
         <v>0.14230000000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:21" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="38" t="s">
         <v>22</v>
       </c>
@@ -5773,7 +5801,7 @@
         <v>0.1598</v>
       </c>
     </row>
-    <row r="70" spans="1:21" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:21" ht="30" x14ac:dyDescent="0.2">
       <c r="A70" s="36" t="s">
         <v>23</v>
       </c>
@@ -5838,7 +5866,7 @@
         <v>0.1807</v>
       </c>
     </row>
-    <row r="71" spans="1:21" ht="28.5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:21" ht="30" x14ac:dyDescent="0.2">
       <c r="A71" s="38" t="s">
         <v>29</v>
       </c>
@@ -5903,7 +5931,7 @@
         <v>0.16539999999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:21" ht="28.5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:21" ht="30" x14ac:dyDescent="0.2">
       <c r="A72" s="36" t="s">
         <v>30</v>
       </c>
@@ -5968,7 +5996,7 @@
         <v>0.1772</v>
       </c>
     </row>
-    <row r="73" spans="1:21" ht="28.5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:21" ht="30" x14ac:dyDescent="0.2">
       <c r="A73" s="38" t="s">
         <v>31</v>
       </c>
@@ -6033,7 +6061,7 @@
         <v>0.19589999999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:21" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:21" ht="30" x14ac:dyDescent="0.2">
       <c r="A74" s="36" t="s">
         <v>32</v>
       </c>
@@ -6098,7 +6126,7 @@
         <v>0.1719</v>
       </c>
     </row>
-    <row r="75" spans="1:21" ht="28.5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:21" ht="30" x14ac:dyDescent="0.2">
       <c r="A75" s="38" t="s">
         <v>24</v>
       </c>
@@ -6163,7 +6191,7 @@
         <v>9.7000000000000003E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:21" ht="28.5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:21" ht="30" x14ac:dyDescent="0.2">
       <c r="A76" s="36" t="s">
         <v>25</v>
       </c>
@@ -6228,7 +6256,7 @@
         <v>3.1899999999999998E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:21" ht="28.5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:21" ht="30" x14ac:dyDescent="0.2">
       <c r="A77" s="38" t="s">
         <v>26</v>
       </c>
@@ -6293,7 +6321,7 @@
         <v>0.12820000000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:21" ht="28.5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:21" ht="30" x14ac:dyDescent="0.2">
       <c r="A78" s="36" t="s">
         <v>28</v>
       </c>
@@ -6358,7 +6386,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:21" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="38" t="s">
         <v>27</v>
       </c>
@@ -6423,7 +6451,7 @@
         <v>4.5600000000000002E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:21" ht="28.5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:21" ht="30" x14ac:dyDescent="0.2">
       <c r="A80" s="36" t="s">
         <v>58</v>
       </c>
@@ -6488,7 +6516,7 @@
         <v>0.12770000000000001</v>
       </c>
     </row>
-    <row r="81" spans="1:21" ht="28.5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:21" ht="30" x14ac:dyDescent="0.2">
       <c r="A81" s="38" t="s">
         <v>33</v>
       </c>
@@ -6553,7 +6581,7 @@
         <v>0.1764</v>
       </c>
     </row>
-    <row r="82" spans="1:21" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A82" s="36" t="s">
         <v>34</v>
       </c>
@@ -6618,7 +6646,7 @@
         <v>0.16789999999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:21" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="40" t="s">
         <v>59</v>
       </c>
@@ -6788,42 +6816,42 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.86328125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="5.86328125" style="4" customWidth="1"/>
-    <col min="3" max="5" width="5.265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="6.73046875" style="4" customWidth="1"/>
-    <col min="11" max="12" width="5.265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="10.86328125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="8.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.86328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" style="4" customWidth="1"/>
+    <col min="3" max="5" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="6.7109375" style="4" customWidth="1"/>
+    <col min="11" max="12" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="10.85546875" style="4" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.73046875" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="9" style="4"/>
-    <col min="23" max="36" width="4.265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.1328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="36" width="4.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="38" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="3" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:20" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="11.65" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="12" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
         <v>39</v>
       </c>
@@ -6847,7 +6875,7 @@
       <c r="S4" s="44"/>
       <c r="T4" s="44"/>
     </row>
-    <row r="5" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -6897,7 +6925,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="30.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
@@ -6947,7 +6975,7 @@
         <v>0.1205</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="30.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>29</v>
       </c>
@@ -6997,7 +7025,7 @@
         <v>0.14180000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="30.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>31</v>
       </c>
@@ -7047,7 +7075,7 @@
         <v>0.17419999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>32</v>
       </c>
@@ -7097,7 +7125,7 @@
         <v>0.1467</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="30.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -7147,7 +7175,7 @@
         <v>0.1462</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="30.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>25</v>
       </c>
@@ -7197,7 +7225,7 @@
         <v>3.09E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="30.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>46</v>
       </c>
@@ -7247,7 +7275,7 @@
         <v>7.0800000000000002E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="30.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>47</v>
       </c>
@@ -7297,7 +7325,7 @@
         <v>0.11600000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>48</v>
       </c>
@@ -7347,7 +7375,7 @@
         <v>0.1638</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="30.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>33</v>
       </c>
@@ -7397,7 +7425,7 @@
         <v>0.15659999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>50</v>
       </c>

</xml_diff>